<commit_message>
Upload to GitHub done.
</commit_message>
<xml_diff>
--- a/data/cash-us.xlsx
+++ b/data/cash-us.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IanMcLean\McLean Capital Dropbox\Ian McLean\_Website + data + articles\___Real CPI website\_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A1A8535-0D2D-425E-B38A-F38A3FBFE800}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10BBB508-3D08-47CD-95B0-6451855C8D68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -93,16 +93,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -409,10 +408,10 @@
       <c r="A2" s="3">
         <v>45627</v>
       </c>
-      <c r="B2" s="4">
-        <v>0.1120754716981132</v>
-      </c>
-      <c r="C2" s="6">
+      <c r="B2" s="5">
+        <v>11.20754716981132</v>
+      </c>
+      <c r="C2" s="4">
         <f>(B2/B3-1)*100</f>
         <v>-6.6037735849056585</v>
       </c>
@@ -421,34 +420,34 @@
       <c r="A3" s="3">
         <v>45261</v>
       </c>
-      <c r="B3" s="5">
-        <v>0.12</v>
-      </c>
-      <c r="C3" s="6">
+      <c r="B3" s="4">
+        <v>12</v>
+      </c>
+      <c r="C3" s="4">
         <f t="shared" ref="C3:C18" si="0">(B3/B4-1)*100</f>
-        <v>-11.926605504587151</v>
+        <v>-11.92660550458714</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>44896</v>
       </c>
-      <c r="B4" s="4">
-        <v>0.13624999999999998</v>
-      </c>
-      <c r="C4" s="6">
-        <f t="shared" si="0"/>
-        <v>-15.384615384615385</v>
+      <c r="B4" s="5">
+        <v>13.624999999999998</v>
+      </c>
+      <c r="C4" s="4">
+        <f t="shared" si="0"/>
+        <v>-15.384615384615397</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>44531</v>
       </c>
-      <c r="B5" s="4">
-        <v>0.16102272727272726</v>
-      </c>
-      <c r="C5" s="6">
+      <c r="B5" s="5">
+        <v>16.102272727272727</v>
+      </c>
+      <c r="C5" s="4">
         <f t="shared" si="0"/>
         <v>-5.9322033898305033</v>
       </c>
@@ -457,34 +456,34 @@
       <c r="A6" s="3">
         <v>44166</v>
       </c>
-      <c r="B6" s="4">
-        <v>0.17117731367731365</v>
-      </c>
-      <c r="C6" s="6">
-        <f t="shared" si="0"/>
-        <v>-2.9126213592232997</v>
+      <c r="B6" s="5">
+        <v>17.117731367731366</v>
+      </c>
+      <c r="C6" s="4">
+        <f t="shared" si="0"/>
+        <v>-2.9126213592232886</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>43800</v>
       </c>
-      <c r="B7" s="4">
-        <v>0.17631263308763306</v>
-      </c>
-      <c r="C7" s="6">
-        <f t="shared" si="0"/>
-        <v>-7.2727272727272751</v>
+      <c r="B7" s="5">
+        <v>17.631263308763305</v>
+      </c>
+      <c r="C7" s="4">
+        <f t="shared" si="0"/>
+        <v>-7.2727272727272858</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>43435</v>
       </c>
-      <c r="B8" s="4">
-        <v>0.19014107489842783</v>
-      </c>
-      <c r="C8" s="6">
+      <c r="B8" s="5">
+        <v>19.014107489842782</v>
+      </c>
+      <c r="C8" s="4">
         <f t="shared" si="0"/>
         <v>-6.3636363636363598</v>
       </c>
@@ -493,10 +492,10 @@
       <c r="A9" s="3">
         <v>43070</v>
       </c>
-      <c r="B9" s="4">
-        <v>0.20306328387210737</v>
-      </c>
-      <c r="C9" s="6">
+      <c r="B9" s="5">
+        <v>20.306328387210737</v>
+      </c>
+      <c r="C9" s="4">
         <f t="shared" si="0"/>
         <v>-6.25</v>
       </c>
@@ -505,34 +504,34 @@
       <c r="A10" s="3">
         <v>42705</v>
       </c>
-      <c r="B10" s="4">
-        <v>0.21660083613024786</v>
-      </c>
-      <c r="C10" s="6">
-        <f t="shared" si="0"/>
-        <v>-3.6363636363636376</v>
+      <c r="B10" s="5">
+        <v>21.660083613024785</v>
+      </c>
+      <c r="C10" s="4">
+        <f t="shared" si="0"/>
+        <v>-3.6363636363636487</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>42339</v>
       </c>
-      <c r="B11" s="4">
-        <v>0.22477445258799306</v>
-      </c>
-      <c r="C11" s="6">
-        <f t="shared" si="0"/>
-        <v>-3.669724770642202</v>
+      <c r="B11" s="5">
+        <v>22.477445258799307</v>
+      </c>
+      <c r="C11" s="4">
+        <f t="shared" si="0"/>
+        <v>-3.6697247706421909</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>41974</v>
       </c>
-      <c r="B12" s="4">
-        <v>0.23333728887705946</v>
-      </c>
-      <c r="C12" s="6">
+      <c r="B12" s="5">
+        <v>23.333728887705945</v>
+      </c>
+      <c r="C12" s="4">
         <f t="shared" si="0"/>
         <v>-3.669724770642202</v>
       </c>
@@ -541,10 +540,10 @@
       <c r="A13" s="3">
         <v>41609</v>
       </c>
-      <c r="B13" s="4">
-        <v>0.24222632845332839</v>
-      </c>
-      <c r="C13" s="6">
+      <c r="B13" s="5">
+        <v>24.222632845332839</v>
+      </c>
+      <c r="C13" s="4">
         <f t="shared" si="0"/>
         <v>-2.8571428571428581</v>
       </c>
@@ -553,10 +552,10 @@
       <c r="A14" s="3">
         <v>41244</v>
       </c>
-      <c r="B14" s="4">
-        <v>0.24935063223136747</v>
-      </c>
-      <c r="C14" s="6">
+      <c r="B14" s="5">
+        <v>24.935063223136748</v>
+      </c>
+      <c r="C14" s="4">
         <f t="shared" si="0"/>
         <v>3.8095238095238182</v>
       </c>
@@ -565,10 +564,10 @@
       <c r="A15" s="3">
         <v>40878</v>
       </c>
-      <c r="B15" s="4">
-        <v>0.24020015031462003</v>
-      </c>
-      <c r="C15" s="6">
+      <c r="B15" s="5">
+        <v>24.020015031462002</v>
+      </c>
+      <c r="C15" s="4">
         <f t="shared" si="0"/>
         <v>-3.5714285714285698</v>
       </c>
@@ -577,10 +576,10 @@
       <c r="A16" s="3">
         <v>40513</v>
       </c>
-      <c r="B16" s="4">
-        <v>0.24909645217812446</v>
-      </c>
-      <c r="C16" s="6">
+      <c r="B16" s="5">
+        <v>24.909645217812447</v>
+      </c>
+      <c r="C16" s="4">
         <f t="shared" si="0"/>
         <v>-9.259259259259256</v>
       </c>
@@ -589,10 +588,10 @@
       <c r="A17" s="3">
         <v>40148</v>
       </c>
-      <c r="B17" s="4">
-        <v>0.27451445750242287</v>
-      </c>
-      <c r="C17" s="6">
+      <c r="B17" s="5">
+        <v>27.451445750242286</v>
+      </c>
+      <c r="C17" s="4">
         <f t="shared" si="0"/>
         <v>-6.9306930693069262</v>
       </c>
@@ -601,20 +600,20 @@
       <c r="A18" s="3">
         <v>39783</v>
       </c>
-      <c r="B18" s="4">
-        <v>0.29495702348664582</v>
-      </c>
-      <c r="C18" s="6">
-        <f t="shared" si="0"/>
-        <v>-4.5045045045045029</v>
+      <c r="B18" s="5">
+        <v>29.495702348664583</v>
+      </c>
+      <c r="C18" s="4">
+        <f t="shared" si="0"/>
+        <v>-4.5045045045044922</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>39417</v>
       </c>
-      <c r="B19" s="4">
-        <v>0.3088700906322423</v>
+      <c r="B19" s="5">
+        <v>30.88700906322423</v>
       </c>
     </row>
   </sheetData>

</xml_diff>